<commit_message>
add test for read date value from test case
</commit_message>
<xml_diff>
--- a/test/sample_etl.syntax.xlsx
+++ b/test/sample_etl.syntax.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
   <si>
     <t>CASE</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>some_int_var</t>
+  </si>
+  <si>
+    <t>data_date</t>
   </si>
   <si>
     <t>UDFS</t>
@@ -112,10 +115,16 @@
     <t>sample.result</t>
   </si>
   <si>
+    <t>2021-01-01</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -772,6 +781,7 @@
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,10 +1043,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="5"/>
@@ -1053,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:4">
+    <row r="3" customHeight="1" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1066,8 +1076,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" customHeight="1" spans="2:4">
+    <row r="4" customHeight="1" spans="2:5">
       <c r="B4">
         <v>1</v>
       </c>
@@ -1076,75 +1089,78 @@
       </c>
       <c r="D4">
         <v>3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>44197</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" ht="24" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="24" spans="2:3">
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" ht="15" spans="2:6">
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="6">
         <v>44197</v>
@@ -1155,19 +1171,19 @@
     </row>
     <row r="16" ht="12" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" ht="12" spans="3:5">
@@ -1175,10 +1191,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="6">
-        <v>44197</v>
+        <v>22</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="3:5">
@@ -1186,11 +1202,20 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="3:5">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>